<commit_message>
Better exception handling. Update spreadsheet
</commit_message>
<xml_diff>
--- a/dek.xlsx
+++ b/dek.xlsx
@@ -5,19 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kal\Source\Repos\keithalewis\xlllapack\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kal\Source\Repos\keithalewis\xlllapack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F758847-9F62-455F-8EE7-676A54C1E5AD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA7EBE63-C0CA-4C0E-A8A4-BFF596A0B226}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13875" xr2:uid="{CB85EF7A-7099-4FC8-997B-E85230279866}"/>
+    <workbookView xWindow="2220" yWindow="1943" windowWidth="15105" windowHeight="9802" xr2:uid="{CB85EF7A-7099-4FC8-997B-E85230279866}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="eigenvalue0">_xll.ARRAY.GET(Sheet1!$C$8)</definedName>
-    <definedName name="interval">_xll.ARRAY.GET(Sheet1!$C$5)</definedName>
+    <definedName name="eigenvalue0">_xll.ARRAY.GET(Sheet1!$C$9)</definedName>
+    <definedName name="interval">_xll.ARRAY.GET(Sheet1!$C$6)</definedName>
+    <definedName name="sin">_xll.ARRAY.GET(Sheet1!$C$11)</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>interval</t>
   </si>
@@ -74,6 +75,15 @@
   </si>
   <si>
     <t>eigenvalue0</t>
+  </si>
+  <si>
+    <t>offset</t>
+  </si>
+  <si>
+    <t>sin</t>
+  </si>
+  <si>
+    <t>max</t>
   </si>
 </sst>
 </file>
@@ -146,6 +156,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Double Exponential Kernel Eigenvectors</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -185,111 +220,355 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
+          <c:dPt>
+            <c:idx val="74"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:ln w="3175">
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-9582-419A-82EF-2E407233FBCF}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:xVal>
             <c:numRef>
               <c:f>[0]!interval</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="100"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.4482758620689655E-2</c:v>
+                  <c:v>1.0101010101010102E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.8965517241379309E-2</c:v>
+                  <c:v>2.0202020202020204E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.10344827586206896</c:v>
+                  <c:v>3.0303030303030304E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.13793103448275862</c:v>
+                  <c:v>4.0404040404040407E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.17241379310344829</c:v>
+                  <c:v>5.0505050505050511E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.20689655172413793</c:v>
+                  <c:v>6.0606060606060608E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.24137931034482757</c:v>
+                  <c:v>7.0707070707070718E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.27586206896551724</c:v>
+                  <c:v>8.0808080808080815E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.31034482758620691</c:v>
+                  <c:v>9.0909090909090912E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.34482758620689657</c:v>
+                  <c:v>0.10101010101010102</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.37931034482758619</c:v>
+                  <c:v>0.11111111111111112</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.41379310344827586</c:v>
+                  <c:v>0.12121212121212122</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.44827586206896552</c:v>
+                  <c:v>0.13131313131313133</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.48275862068965514</c:v>
+                  <c:v>0.14141414141414144</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.51724137931034486</c:v>
+                  <c:v>0.15151515151515152</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.55172413793103448</c:v>
+                  <c:v>0.16161616161616163</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.58620689655172409</c:v>
+                  <c:v>0.17171717171717174</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.62068965517241381</c:v>
+                  <c:v>0.18181818181818182</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.65517241379310343</c:v>
+                  <c:v>0.19191919191919193</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.68965517241379315</c:v>
+                  <c:v>0.20202020202020204</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.72413793103448276</c:v>
+                  <c:v>0.21212121212121213</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.75862068965517238</c:v>
+                  <c:v>0.22222222222222224</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.7931034482758621</c:v>
+                  <c:v>0.23232323232323235</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.82758620689655171</c:v>
+                  <c:v>0.24242424242424243</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.86206896551724133</c:v>
+                  <c:v>0.25252525252525254</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.89655172413793105</c:v>
+                  <c:v>0.26262626262626265</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.93103448275862066</c:v>
+                  <c:v>0.27272727272727276</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.96551724137931028</c:v>
+                  <c:v>0.28282828282828287</c:v>
                 </c:pt>
                 <c:pt idx="29">
+                  <c:v>0.29292929292929293</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.30303030303030304</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.31313131313131315</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.32323232323232326</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.33333333333333337</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.34343434343434348</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.35353535353535359</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.36363636363636365</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.37373737373737376</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.38383838383838387</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.39393939393939398</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.40404040404040409</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.4141414141414142</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.42424242424242425</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.43434343434343436</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.44444444444444448</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.45454545454545459</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.4646464646464647</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.47474747474747481</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.48484848484848486</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.49494949494949497</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.50505050505050508</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.51515151515151525</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.5252525252525253</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.53535353535353536</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.54545454545454553</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.55555555555555558</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.56565656565656575</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.5757575757575758</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.58585858585858586</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.59595959595959602</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.60606060606060608</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.61616161616161624</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.6262626262626263</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.63636363636363646</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.64646464646464652</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.65656565656565657</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.66666666666666674</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.6767676767676768</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.68686868686868696</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.69696969696969702</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.70707070707070718</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.71717171717171724</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.72727272727272729</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.73737373737373746</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.74747474747474751</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.75757575757575768</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.76767676767676774</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.77777777777777779</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.78787878787878796</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.79797979797979801</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.80808080808080818</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.81818181818181823</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.8282828282828284</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.83838383838383845</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.84848484848484851</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.85858585858585867</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.86868686868686873</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.8787878787878789</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.88888888888888895</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.89898989898989912</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.90909090909090917</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.91919191919191923</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.92929292929292939</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.93939393939393945</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.94949494949494961</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.95959595959595967</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.96969696969696972</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.97979797979797989</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.98989898989898994</c:v>
+                </c:pt>
+                <c:pt idx="99">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -300,96 +579,303 @@
               <c:f>[0]!eigenvalue0</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="99"/>
                 <c:pt idx="0">
-                  <c:v>-1.3734190181916741E-2</c:v>
+                  <c:v>-8.9240907204290957E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.05867482533133E-2</c:v>
+                  <c:v>2.6541859538716645E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-6.6995140049187718E-2</c:v>
+                  <c:v>-4.3741089653146686E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.2670361952855565E-2</c:v>
+                  <c:v>6.0250566326856339E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.11733143388623912</c:v>
+                  <c:v>-7.580995154813977E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.14070847425136859</c:v>
+                  <c:v>9.017388930117623E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.16254565341412569</c:v>
+                  <c:v>-0.10311587458659269</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.18260399340861053</c:v>
+                  <c:v>0.11443182517996615</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.20066398322309953</c:v>
+                  <c:v>-0.12394329980532102</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.21652798104690291</c:v>
+                  <c:v>0.13150031197635492</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.23002237718882565</c:v>
+                  <c:v>-0.13698369513400768</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.24099949399704845</c:v>
+                  <c:v>0.14030698178449699</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-0.24933920198842693</c:v>
+                  <c:v>-0.14141776700562358</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.25495023450085857</c:v>
+                  <c:v>0.14029853482021071</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-0.25777118648167768</c:v>
+                  <c:v>-0.13696693440563407</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.25777118648172448</c:v>
+                  <c:v>0.1314755017838618</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-0.25495023450099968</c:v>
+                  <c:v>-0.1239108313807038</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.24933920198865997</c:v>
+                  <c:v>0.11439221051792568</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-0.2409994939973675</c:v>
+                  <c:v>-0.10306973837088897</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.23002237718922608</c:v>
+                  <c:v>9.012195905399005E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-0.21652798104737481</c:v>
+                  <c:v>-7.5753046157754966E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.20066398322362422</c:v>
+                  <c:v>6.018958313455218E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-0.18260399340917297</c:v>
+                  <c:v>-4.3676990303072462E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.16254565341471638</c:v>
+                  <c:v>2.6475654814226843E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-0.14070847425197899</c:v>
+                  <c:v>-8.8568246050131569E-3</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.11733143388685709</c:v>
+                  <c:v>-8.9016689114055688E-3</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-9.2670361953468713E-2</c:v>
+                  <c:v>2.6519791970542342E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>6.6995140049787003E-2</c:v>
+                  <c:v>-4.3719724310313735E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-4.0586748253809382E-2</c:v>
+                  <c:v>6.023024011999039E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.3734190182119315E-2</c:v>
+                  <c:v>-7.5790985001229536E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>9.0156581497721378E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-0.10310049845342216</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.11441862318342259</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-0.12393248012774286</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.13149204523326091</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-0.13697811168371959</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.14030416967250789</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-0.14141777057615429</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.14030135401696658</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-0.13697252477273938</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.13148377516684559</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-0.12392165731657358</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.1144054182924354</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-0.1030851197105629</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>9.0139271410390839E-2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-7.5772016532193662E-2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>6.0209912383040812E-2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-4.3698357853601079E-2</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2.6497723721864222E-2</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-8.8792468651254335E-3</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>-8.879246875527904E-3</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2.6497723732101575E-2</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>-4.3698357863437252E-2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>6.0209912392271678E-2</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>-7.5772016540749387E-2</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>9.0139271418282207E-2</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>-0.10308511971780047</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.11440541829896841</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>-0.12392165732232367</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.13148377517177115</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>-0.13697252477684299</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.14030135402026048</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>-0.14141777057864122</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.14030416967415721</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>-0.13697811168442087</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.13149204523295602</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>-0.1239324801265142</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.1144186231813781</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>-0.10310049845059294</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>9.0156581494081692E-2</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>-7.5790984996859406E-2</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>6.0230240115067626E-2</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>-4.3719724304981937E-2</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>2.6519791964936326E-2</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>-8.9016689056607718E-3</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>-8.8568246108365577E-3</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>2.6475654820103826E-2</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>-4.3676990308959739E-2</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>6.0189583140403846E-2</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>-7.5753046163511278E-2</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>9.0121959059599632E-2</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>-0.10306973837633651</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.11439221052327943</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>-0.12391083138602978</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.13147550178915438</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>-0.13696693441093594</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.14029853482553975</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>-0.14141776701085637</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.14030698178945974</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>-0.13698369513863454</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.13150031198063317</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>-0.12394329980911403</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.1144318251831366</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>-0.10311587458916534</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>9.0173889303194851E-2</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>-7.5809951549545979E-2</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>6.0250566327486793E-2</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>-4.374108965279673E-2</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>2.6541859537781643E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -398,6 +884,656 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-398A-4BA7-8BC4-655E6B5E2463}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="3175">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>[0]!interval</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0101010101010102E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0202020202020204E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0303030303030304E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0404040404040407E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0505050505050511E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.0606060606060608E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.0707070707070718E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.0808080808080815E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.0909090909090912E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.10101010101010102</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.11111111111111112</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.12121212121212122</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.13131313131313133</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.14141414141414144</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.15151515151515152</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.16161616161616163</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.17171717171717174</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.18181818181818182</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.19191919191919193</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.20202020202020204</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.21212121212121213</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.22222222222222224</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.23232323232323235</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.24242424242424243</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.25252525252525254</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.26262626262626265</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.27272727272727276</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.28282828282828287</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.29292929292929293</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.30303030303030304</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.31313131313131315</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.32323232323232326</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.33333333333333337</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.34343434343434348</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.35353535353535359</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.36363636363636365</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.37373737373737376</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.38383838383838387</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.39393939393939398</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.40404040404040409</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.4141414141414142</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.42424242424242425</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.43434343434343436</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.44444444444444448</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.45454545454545459</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.4646464646464647</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.47474747474747481</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.48484848484848486</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.49494949494949497</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.50505050505050508</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.51515151515151525</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.5252525252525253</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.53535353535353536</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.54545454545454553</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.55555555555555558</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.56565656565656575</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.5757575757575758</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.58585858585858586</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.59595959595959602</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.60606060606060608</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.61616161616161624</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.6262626262626263</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.63636363636363646</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.64646464646464652</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.65656565656565657</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.66666666666666674</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.6767676767676768</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.68686868686868696</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.69696969696969702</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.70707070707070718</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.71717171717171724</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.72727272727272729</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.73737373737373746</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.74747474747474751</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.75757575757575768</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.76767676767676774</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.77777777777777779</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.78787878787878796</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.79797979797979801</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.80808080808080818</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.81818181818181823</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.8282828282828284</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.83838383838383845</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.84848484848484851</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.85858585858585867</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.86868686868686873</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.8787878787878789</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.88888888888888895</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.89898989898989912</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.90909090909090917</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.91919191919191923</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.92929292929292939</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.93939393939393945</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.94949494949494961</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.95959595959595967</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.96969696969696972</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.97979797979797989</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.98989898989898994</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>[0]!sin</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7761805078255068E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.5237816063875153E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.2146837398159465E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.8216796598143226E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.3189122004695734E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.6822903297309054E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.1088987678313371</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.11922241042596737</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.12762771980731633</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.13397945140100798</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.13817540346800267</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.14014806156883641</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.13986568489622517</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.1373328169965356</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.13259021266242355</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.12571418217296376</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.11681536343269398</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.10603694176631487</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.3552346013215618E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7.9562457992527244E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6.4292380239455271E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.7987814021222978E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.0911105911707294E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.3337026536858084E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-4.4516505875305968E-3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-2.2168698987542049E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-3.9529044722248427E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-5.6253353330134169E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-7.2072524425147069E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-8.6732021622645358E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-9.999596812510822E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-0.11165094206810643</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-0.12150941055799278</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-0.12941274714636153</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-0.13523378418898338</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-0.1388788590208048</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-0.14028932102329034</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-0.13944247533482981</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-0.13635194801955747</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-0.13106746681887907</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-0.12367406101349793</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-0.11429069327045831</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-0.10306834548930063</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-9.018758944677957E-2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-7.5855681329381142E-2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-6.0303226903697785E-2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-4.3780470983319886E-2</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-2.6553270896108729E-2</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-8.8988187402697563E-3</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>8.8988187402698118E-3</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2.6553270896108785E-2</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>4.3780470983320052E-2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>6.0303226903697833E-2</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>7.5855681329381183E-2</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>9.0187589446779612E-2</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.10306834548930074</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.11429069327045834</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.1236740610134979</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.13106746681887915</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.1363519480195575</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.13944247533482984</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.14028932102329034</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.1388788590208048</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.13523378418898335</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.12941274714636153</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.12150941055799271</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.1116509420681064</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>9.9995968125108053E-2</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>8.6732021622645414E-2</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>7.2072524425147028E-2</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>5.6253353330134058E-2</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>3.9529044722248434E-2</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>2.2168698987541868E-2</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>4.451650587530478E-3</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>-1.3337026536858077E-2</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>-3.0911105911707291E-2</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>-4.7987814021222909E-2</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>-6.4292380239455313E-2</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>-7.95624579925273E-2</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>-9.3552346013215743E-2</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>-0.10603694176631495</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>-0.11681536343269405</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>-0.12571418217296376</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>-0.13259021266242352</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>-0.13733281699653563</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>-0.13986568489622517</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>-0.14014806156883639</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>-0.13817540346800264</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>-0.13397945140100792</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>-0.12762771980731633</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>-0.11922241042596739</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>-0.10889876783133699</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>-9.6822903297309013E-2</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>-8.3189122004695512E-2</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>-6.8216796598143281E-2</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>-5.2146837398159569E-2</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>-3.5237816063875091E-2</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>-1.7761805078255071E-2</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>-6.87587527808994E-17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9582-419A-82EF-2E407233FBCF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1157,8 +2293,8 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>311943</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>140493</xdr:rowOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>38270</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1483,10 +2619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6351286F-66CB-44D7-804F-03E59B919781}">
-  <dimension ref="B2:C8"/>
+  <dimension ref="B2:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1509,43 +2645,69 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>30</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B5" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
-      <c r="C5" cm="1">
-        <f t="array" ref="C5">_xll.ARRAY.SET(_xll.ARRAY.INTERVAL(C2,C3,C4))</f>
-        <v>2256622</v>
+      <c r="C5">
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B6" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" cm="1">
-        <f t="array" ref="C6">_xll.ARRAY.SET(_xll.ARRAY.APPLY(_xll.DEK,_xll.ARRAY.GET(C5),_xll.ARRAY.GET(C5)))</f>
-        <v>2256634</v>
+        <f t="array" ref="C6">_xll.ARRAY.SET(_xll.ARRAY.INTERVAL(C2,C3,C4))</f>
+        <v>-1360338</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B7" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" cm="1">
-        <f t="array" ref="C7">_xll.ARRAY.SET(_xll.SYEV(_xll.ARRAY.GET(C6),TRUE))</f>
-        <v>2256502</v>
+        <f t="array" ref="C7">_xll.ARRAY.SET(_xll.ARRAY.APPLY(_xll.DEK,_xll.ARRAY.GET(C6),_xll.ARRAY.GET(C6)))</f>
+        <v>-1360230</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" cm="1">
+        <f t="array" ref="C8">_xll.ARRAY.SET(_xll.SYEV(_xll.ARRAY.GET(C7),TRUE))</f>
+        <v>-1360206</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C8" cm="1">
-        <f t="array" ref="C8">_xll.ARRAY.SET(_xll.ARRAY.SLICE(_xll.ARRAY.GET(C7),C4,C4))</f>
-        <v>2256562</v>
+      <c r="C9" cm="1">
+        <f t="array" ref="C9">_xll.ARRAY.SET(_xll.ARRAY.SLICE(_xll.ARRAY.GET(C8),C4+C5,C4))</f>
+        <v>-1360278</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <f>MAX(_xll.ARRAY.GET(C9))</f>
+        <v>0.14030698178945974</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" cm="1">
+        <f t="array" ref="C11">_xll.ARRAY.SET(C10*SIN((C5+1)*PI()*_xll.ARRAY.GET(C6)))</f>
+        <v>-1360254</v>
       </c>
     </row>
   </sheetData>

</xml_diff>